<commit_message>
Power test board updates
</commit_message>
<xml_diff>
--- a/Electrical/Test Boards/Power_Breakout/BOM.xlsx
+++ b/Electrical/Test Boards/Power_Breakout/BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Designator:</t>
   </si>
@@ -98,19 +98,19 @@
     <t>D2</t>
   </si>
   <si>
-    <t>MBRS130L</t>
+    <t>1N5819HW-7-F</t>
   </si>
   <si>
     <t>Switching Regulator Schottky Diode</t>
   </si>
   <si>
-    <t>http://www.fairchildsemi.com/datasheets/MB/MBRS130L.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/fairchild-semiconductor/MBRS130L/MBRS130LFSCT-ND/3042645</t>
-  </si>
-  <si>
-    <t>http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/MBRS130L/?qs=3csLVnQQLU2Pf2cVoQKtiA==</t>
+    <t>http://www.diodes.com/_files/datasheets/ds30217.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/diodes-incorporated/1N5819HW-7-F/1N5819HW-FDICT-ND/815283</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N5819HW-7-F/?qs=NQ47qNm99eDyWTEd07miYA==</t>
   </si>
   <si>
     <t>D3</t>
@@ -134,7 +134,16 @@
     <t>R1</t>
   </si>
   <si>
-    <t>MOSFET Resistor</t>
+    <t>CF14JT100K</t>
+  </si>
+  <si>
+    <t>MOSFET Resistor, 100K Ohm</t>
+  </si>
+  <si>
+    <t>http://www.seielect.com/catalog/SEI-CF_CFM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100K/CF14JT100KCT-ND/1830399</t>
   </si>
   <si>
     <t>R2</t>
@@ -143,7 +152,7 @@
     <t>ERJ-3EKF1000V</t>
   </si>
   <si>
-    <t>PWR LED Resistor (100 Ohm), 0603</t>
+    <t>PWR LED Resistor, 100 Ohm, 0603</t>
   </si>
   <si>
     <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW</t>
@@ -182,7 +191,7 @@
     <t>68uF Input Bypass Capacitor</t>
   </si>
   <si>
-    <t>http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+ABA0114+EEEFPV680XAP+7+WW</t>
+    <t>http://industrial.panasonic.com/cdbs/www-data/pdf/RDE0000/ABA0000C1184.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-FPV680XAP/PCE4553CT-ND/1701052</t>
@@ -194,10 +203,19 @@
     <t>C2</t>
   </si>
   <si>
-    <t>Output Capacitor</t>
-  </si>
-  <si>
-    <t>C3</t>
+    <t>TPSD107K016R0125</t>
+  </si>
+  <si>
+    <t>Output Capacitor, 100uF</t>
+  </si>
+  <si>
+    <t>http://datasheets.avx.com/tps.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/avx-corporation/TPSD107K016R0125/478-1778-1-ND/564810</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/AVX/TPSD107K016R0125/?qs=Ow%2BOiPmaljGaFh%2BHI/q%2BNg==</t>
   </si>
   <si>
     <t>L1</t>
@@ -221,7 +239,37 @@
     <t>S1</t>
   </si>
   <si>
+    <t>GF-123-0054</t>
+  </si>
+  <si>
     <t>Power Switch</t>
+  </si>
+  <si>
+    <t>https://media.digikey.com/pdf/Data Sheets/CW Industries PDFs/GF-123-0054_Dwg.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/cw-industries/GF-123-0054/CWI333-ND/4089770</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/CW-Industries/GF-123-0054/?qs=n1d6TrdN4SA9FY9ssLiRzw==</t>
+  </si>
+  <si>
+    <t>TP1,2,3,4</t>
+  </si>
+  <si>
+    <t>RCS-0C</t>
+  </si>
+  <si>
+    <t>Test Point</t>
+  </si>
+  <si>
+    <t>http://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=1773266&amp;DocType=DS&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/RCS-0C/A106143CT-ND/3477800</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/RCS-0C/?qs=ip69W3eHERVjlVbETUUe0w==</t>
   </si>
   <si>
     <t>SQP500JB-6R8</t>
@@ -346,7 +394,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -387,10 +435,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -419,7 +463,7 @@
   <dimension ref="A1:AMI65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>
@@ -1578,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="n">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>27</v>
@@ -1638,14 +1682,20 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>0.37</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
       <c r="AMH7" s="0"/>
@@ -1653,28 +1703,28 @@
     </row>
     <row r="8" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I8" s="9"/>
       <c r="AMH8" s="0"/>
@@ -1682,7 +1732,7 @@
     </row>
     <row r="9" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>1</v>
@@ -1691,19 +1741,19 @@
         <v>0.18</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I9" s="0"/>
       <c r="K9" s="1"/>
@@ -1713,7 +1763,7 @@
     </row>
     <row r="10" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
@@ -1722,102 +1772,128 @@
         <v>0.89</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B11" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D11" s="7"/>
+        <v>1.39</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="E11" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="I11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="6" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="9"/>
+        <v>3.24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="I12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B13" s="5" t="n">
         <v>1</v>
       </c>
       <c r="C13" s="6" t="n">
-        <v>3.24</v>
+        <v>0.93</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="I13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C14" s="6" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>0.16</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="E14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
+        <v>81</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="I14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1829,32 +1905,32 @@
         <v>0.56</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="6"/>
       <c r="H16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="17.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12" t="s">
-        <v>73</v>
+      <c r="B17" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="C17" s="6" t="n">
-        <f aca="false">(C2*B2)+(C3*B3)+(C4*B4)+(C5*B5)+(C6*B6)+(C7*B7)+(C8*B8)+(C9*B9)+(C10*B10)+(C11*B11)+(C12*B12)+(C13*B13)+(C14*B14)</f>
-        <v>11.83</v>
+        <f aca="false">(C2*B2)+(C3*B3)+(C4*B4)+(C5*B5)+(C6*B6)+(C7*B7)+(C8*B8)+(C9*B9)+(C10*B10)+(C11*B11)+(C12*B12)+(C13*B13)+(C14*B14)+(C15*B15)</f>
+        <v>14.59</v>
       </c>
       <c r="H17" s="4"/>
     </row>
@@ -1871,26 +1947,37 @@
     <hyperlink ref="F4" r:id="rId7" display="http://www.fairchildsemi.com/datasheets/1N/1N4731A.pdf"/>
     <hyperlink ref="G4" r:id="rId8" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/1N4749A_T50A/1N4749A_T50AFSCT-ND/3478158"/>
     <hyperlink ref="H4" r:id="rId9" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/1N4749A_T50A/?qs=9h%2BT/FFCxR/U89fjfSyrjQ=="/>
-    <hyperlink ref="F5" r:id="rId10" display="http://www.fairchildsemi.com/datasheets/MB/MBRS130L.pdf"/>
-    <hyperlink ref="G5" r:id="rId11" display="https://www.digikey.com/product-detail/en/fairchild-semiconductor/MBRS130L/MBRS130LFSCT-ND/3042645"/>
-    <hyperlink ref="H5" r:id="rId12" display="http://www.mouser.com/ProductDetail/Fairchild-Semiconductor/MBRS130L/?qs=3csLVnQQLU2Pf2cVoQKtiA=="/>
+    <hyperlink ref="F5" r:id="rId10" display="http://www.diodes.com/_files/datasheets/ds30217.pdf"/>
+    <hyperlink ref="G5" r:id="rId11" display="https://www.digikey.com/product-detail/en/diodes-incorporated/1N5819HW-7-F/1N5819HW-FDICT-ND/815283"/>
+    <hyperlink ref="H5" r:id="rId12" display="http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N5819HW-7-F/?qs=NQ47qNm99eDyWTEd07miYA=="/>
     <hyperlink ref="F6" r:id="rId13" display="https://media.digikey.com/pdf/Data Sheets/Osram PDFs/LB_LT Q39G.pdf"/>
     <hyperlink ref="G6" r:id="rId14" display="https://www.digikey.com/product-detail/en/osram-opto-semiconductors-inc/LB-Q39G-L2OO-35-1/475-2816-1-ND/2176355"/>
     <hyperlink ref="H6" r:id="rId15" display="http://www.mouser.com/ProductDetail/Osram-Opto-Semiconductor/LB-Q39G-L2OO-35-1/?qs=/ha2pyFadugdwYCal9BdM9SWhVbJU5uqsKvsYGbR4IvEO9KLCpls7BBaJhTRZMg6"/>
-    <hyperlink ref="F8" r:id="rId16" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
-    <hyperlink ref="G8" r:id="rId17" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
-    <hyperlink ref="H8" r:id="rId18" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g=="/>
-    <hyperlink ref="F9" r:id="rId19" display="http://www.belfuse.com/pdfs/0ZCJ.pdf"/>
-    <hyperlink ref="G9" r:id="rId20" display="https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312"/>
-    <hyperlink ref="H9" r:id="rId21" display="http://www.mouser.com/ProductDetail/Bel-Fuse/0ZCJ0050AF2E/?qs=SRYZG9HaIQ3Oqm1PQp276Q=="/>
-    <hyperlink ref="F10" r:id="rId22" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+ABA0114+EEEFPV680XAP+7+WW"/>
-    <hyperlink ref="G10" r:id="rId23" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-FPV680XAP/PCE4553CT-ND/1701052"/>
-    <hyperlink ref="H10" r:id="rId24" display="http://www.mouser.com/ProductDetail/Panasonic/EEE-FPV680XAP/?qs=d1CqaRUMZD%2BB3QneHdz%2BNA=="/>
-    <hyperlink ref="F13" r:id="rId25" display="http://productfinder.pulseeng.com/products/datasheets/SPM2007_47.pdf"/>
-    <hyperlink ref="G13" r:id="rId26" display="https://www.digikey.com/product-detail/en/pulse-electronics-corporation/PE-53820SNL/553-1403-ND/1037014"/>
-    <hyperlink ref="H13" r:id="rId27" display="http://www.mouser.com/ProductDetail/Pulse/PE-53820SNL/?qs=sGAEpiMZZMsg%2By3WlYCkU6/kcGZFUWykAerZ435ceU4="/>
-    <hyperlink ref="F15" r:id="rId28" display="http://www.yageo.com/documents/recent/Yageo LR_SQP NSP_2013.pdf"/>
-    <hyperlink ref="G15" r:id="rId29" display="https://www.digikey.com/product-detail/en/yageo/SQP500JB-6R8/6.8W-5-ND/18651"/>
+    <hyperlink ref="F7" r:id="rId16" display="http://www.seielect.com/catalog/SEI-CF_CFM.pdf"/>
+    <hyperlink ref="G7" r:id="rId17" display="https://www.digikey.com/product-detail/en/stackpole-electronics-inc/CF14JT100K/CF14JT100KCT-ND/1830399"/>
+    <hyperlink ref="F8" r:id="rId18" display="http://industrial.panasonic.com/www-cgi/jvcr13pz.cgi?E+PZ+3+AOA0002+ERJ3EKF1000V+7+WW"/>
+    <hyperlink ref="G8" r:id="rId19" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/ERJ-3EKF1000V/P100HCT-ND/198109"/>
+    <hyperlink ref="H8" r:id="rId20" display="http://www.mouser.com/ProductDetail/Panasonic/ERJ-3EKF1000V/?qs=/ha2pyFaduglTbPDDZSypXi%2B1JYi5TJRT2R7dib9ms/8H45gLlep/g=="/>
+    <hyperlink ref="F9" r:id="rId21" display="http://www.belfuse.com/pdfs/0ZCJ.pdf"/>
+    <hyperlink ref="G9" r:id="rId22" display="https://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312"/>
+    <hyperlink ref="H9" r:id="rId23" display="http://www.mouser.com/ProductDetail/Bel-Fuse/0ZCJ0050AF2E/?qs=SRYZG9HaIQ3Oqm1PQp276Q=="/>
+    <hyperlink ref="F10" r:id="rId24" display="http://industrial.panasonic.com/cdbs/www-data/pdf/RDE0000/ABA0000C1184.pdf"/>
+    <hyperlink ref="G10" r:id="rId25" display="https://www.digikey.com/product-detail/en/panasonic-electronic-components/EEE-FPV680XAP/PCE4553CT-ND/1701052"/>
+    <hyperlink ref="H10" r:id="rId26" display="http://www.mouser.com/ProductDetail/Panasonic/EEE-FPV680XAP/?qs=d1CqaRUMZD%2BB3QneHdz%2BNA=="/>
+    <hyperlink ref="F11" r:id="rId27" display="http://datasheets.avx.com/tps.pdf"/>
+    <hyperlink ref="G11" r:id="rId28" display="https://www.digikey.com/product-detail/en/avx-corporation/TPSD107K016R0125/478-1778-1-ND/564810"/>
+    <hyperlink ref="H11" r:id="rId29" display="http://www.mouser.com/ProductDetail/AVX/TPSD107K016R0125/?qs=Ow%2BOiPmaljGaFh%2BHI/q%2BNg=="/>
+    <hyperlink ref="F12" r:id="rId30" display="http://productfinder.pulseeng.com/products/datasheets/SPM2007_47.pdf"/>
+    <hyperlink ref="G12" r:id="rId31" display="https://www.digikey.com/product-detail/en/pulse-electronics-corporation/PE-53820SNL/553-1403-ND/1037014"/>
+    <hyperlink ref="H12" r:id="rId32" display="http://www.mouser.com/ProductDetail/Pulse/PE-53820SNL/?qs=sGAEpiMZZMsg%2By3WlYCkU6/kcGZFUWykAerZ435ceU4="/>
+    <hyperlink ref="F13" r:id="rId33" display="https://media.digikey.com/pdf/Data Sheets/CW Industries PDFs/GF-123-0054_Dwg.pdf"/>
+    <hyperlink ref="G13" r:id="rId34" display="https://www.digikey.com/product-detail/en/cw-industries/GF-123-0054/CWI333-ND/4089770"/>
+    <hyperlink ref="H13" r:id="rId35" display="http://www.mouser.com/ProductDetail/CW-Industries/GF-123-0054/?qs=n1d6TrdN4SA9FY9ssLiRzw=="/>
+    <hyperlink ref="F14" r:id="rId36" display="http://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=1773266&amp;DocType=DS&amp;DocLang=English"/>
+    <hyperlink ref="G14" r:id="rId37" display="https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/RCS-0C/A106143CT-ND/3477800"/>
+    <hyperlink ref="H14" r:id="rId38" display="http://www.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/RCS-0C/?qs=ip69W3eHERVjlVbETUUe0w=="/>
+    <hyperlink ref="F15" r:id="rId39" display="http://www.yageo.com/documents/recent/Yageo LR_SQP NSP_2013.pdf"/>
+    <hyperlink ref="G15" r:id="rId40" display="https://www.digikey.com/product-detail/en/yageo/SQP500JB-6R8/6.8W-5-ND/18651"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Power test board corrections
</commit_message>
<xml_diff>
--- a/Electrical/Test Boards/Power_Breakout/BOM.xlsx
+++ b/Electrical/Test Boards/Power_Breakout/BOM.xlsx
@@ -227,7 +227,7 @@
     <t>PE-53820SNL</t>
   </si>
   <si>
-    <t>100uH Inductor</t>
+    <t>115uH Inductor</t>
   </si>
   <si>
     <t>http://productfinder.pulseeng.com/products/datasheets/SPM2007_47.pdf</t>
@@ -487,7 +487,7 @@
   <dimension ref="A1:AMI65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35"/>

</xml_diff>